<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T07:49:07.522Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -399,13 +399,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Order ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Flat No</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Items</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Total</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Payment</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Collection Date</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Collection Time</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Notes</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Cancel Reason</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Feedback</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>27</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-01-21 07:49</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Renu</v>
+      </c>
+      <c r="D2" t="str">
+        <v>A-1005 Kakkad la vida</v>
+      </c>
+      <c r="E2" t="str">
+        <v>8806022013</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Appe Chutney x1, Vermicelli Kheer x1</v>
+      </c>
+      <c r="G2">
+        <v>110</v>
+      </c>
+      <c r="H2" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I2" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J2" t="str">
+        <v>2026-01-21</v>
+      </c>
+      <c r="K2" t="str">
+        <v>18:30</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Less spicy</v>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -445,10 +534,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -463,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -478,13 +567,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Item</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Quantity Ordered</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Revenue</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Appe Chutney</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Vermicelli Kheer</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T10:01:49.771Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-21 07:49</v>
+        <v>2026-01-21 10:01</v>
       </c>
       <c r="C2" t="str">
-        <v>Renu</v>
+        <v>Vipula Thakkar</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1005 Kakkad la vida</v>
+        <v>B-903, Kakkad lavida</v>
       </c>
       <c r="E2" t="str">
-        <v>8806022013</v>
+        <v>8109861246</v>
       </c>
       <c r="F2" t="str">
-        <v>Appe Chutney x1, Vermicelli Kheer x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G2">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -480,10 +480,10 @@
         <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v>18:30</v>
+        <v/>
       </c>
       <c r="L2" t="str">
-        <v>Less spicy</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -492,9 +492,53 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>27</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-21 07:49</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Renu</v>
+      </c>
+      <c r="D3" t="str">
+        <v>A-1005 Kakkad la vida</v>
+      </c>
+      <c r="E3" t="str">
+        <v>8806022013</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Appe Chutney x1, Vermicelli Kheer x1</v>
+      </c>
+      <c r="G3">
+        <v>110</v>
+      </c>
+      <c r="H3" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
+        <v>2026-01-21</v>
+      </c>
+      <c r="K3" t="str">
+        <v>18:30</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Less spicy</v>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -534,10 +578,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -552,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -588,10 +632,10 @@
         <v>Appe Chutney</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T10:46:28.099Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -471,7 +471,7 @@
         <v>60</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T10:46:47.431Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -474,7 +474,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-21</v>
@@ -599,7 +599,7 @@
         <v>170</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T13:13:36.197Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -515,7 +515,7 @@
         <v>110</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>READY</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -581,13 +581,13 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T13:14:54.106Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -515,7 +515,7 @@
         <v>110</v>
       </c>
       <c r="H3" t="str">
-        <v>READY</v>
+        <v>COOKING</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -584,10 +584,10 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T13:15:00.199Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -515,7 +515,7 @@
         <v>110</v>
       </c>
       <c r="H3" t="str">
-        <v>COOKING</v>
+        <v>READY</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -584,10 +584,10 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-21.xlsx - 2026-01-21T15:28:13.505Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-21.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-21.xlsx
@@ -515,7 +515,7 @@
         <v>110</v>
       </c>
       <c r="H3" t="str">
-        <v>READY</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -587,10 +587,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>